<commit_message>
add Item Config And So on
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/ConsumeData.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/ConsumeData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NF\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,19 +80,64 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AwardProperty_Gold_10002</t>
+  </si>
+  <si>
+    <t>AwardProperty_Gold_10003</t>
+  </si>
+  <si>
+    <t>AwardProperty_Gold_10004</t>
+  </si>
+  <si>
+    <t>AwardProperty_Gold_10005</t>
+  </si>
+  <si>
+    <t>AwardProperty_Gold_10006</t>
+  </si>
+  <si>
     <t>AwardProperty_Gold_10001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Money</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>AwardProperty_Money_10002</t>
+  </si>
+  <si>
+    <t>AwardProperty_Money_10003</t>
+  </si>
+  <si>
+    <t>AwardProperty_Money_10004</t>
+  </si>
+  <si>
+    <t>AwardProperty_Money_10005</t>
+  </si>
+  <si>
+    <t>AwardProperty_Money_10006</t>
+  </si>
+  <si>
+    <t>AwardProperty_SP_10002</t>
+  </si>
+  <si>
+    <t>AwardProperty_SP_10003</t>
+  </si>
+  <si>
+    <t>AwardProperty_SP_10004</t>
+  </si>
+  <si>
+    <t>AwardProperty_SP_10005</t>
+  </si>
+  <si>
+    <t>AwardProperty_SP_10006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -96,6 +146,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -140,7 +197,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -148,6 +205,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -524,40 +584,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.375" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="27.77734375" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" customWidth="1"/>
-    <col min="12" max="12" width="32.77734375" customWidth="1"/>
-    <col min="13" max="14" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="20.25" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="27.75" customWidth="1"/>
+    <col min="11" max="11" width="17.75" customWidth="1"/>
+    <col min="12" max="12" width="32.75" customWidth="1"/>
+    <col min="13" max="14" width="20.25" customWidth="1"/>
     <col min="15" max="15" width="24" customWidth="1"/>
-    <col min="16" max="17" width="21.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.21875" customWidth="1"/>
+    <col min="16" max="17" width="21.5" customWidth="1"/>
+    <col min="18" max="18" width="15.25" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" customWidth="1"/>
+    <col min="20" max="20" width="16.5" customWidth="1"/>
     <col min="21" max="21" width="19" customWidth="1"/>
-    <col min="22" max="22" width="15.21875" customWidth="1"/>
-    <col min="23" max="23" width="20.21875" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" customWidth="1"/>
-    <col min="25" max="25" width="20.21875" customWidth="1"/>
-    <col min="26" max="27" width="17.77734375" customWidth="1"/>
+    <col min="22" max="22" width="15.25" customWidth="1"/>
+    <col min="23" max="23" width="20.25" customWidth="1"/>
+    <col min="24" max="24" width="11.625" customWidth="1"/>
+    <col min="25" max="25" width="20.25" customWidth="1"/>
+    <col min="26" max="27" width="17.75" customWidth="1"/>
     <col min="28" max="28" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,10 +640,10 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -635,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -661,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -687,317 +747,599 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>900</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1300</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1700</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>2100</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
         <v>100</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>500</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>900</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1300</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1700</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>2100</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="D61" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update for new excel format
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/ConsumeData.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/ConsumeData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19455" windowHeight="9990"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -114,10 +114,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -134,17 +134,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -170,54 +164,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,9 +193,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,7 +203,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,31 +217,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,43 +312,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,133 +468,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,11 +601,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,21 +636,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,15 +664,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -690,6 +681,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -703,148 +703,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -940,7 +940,7 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1293,13 +1293,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="28.1083333333333" customWidth="1"/>
     <col min="2" max="3" width="9.33333333333333" customWidth="1"/>
@@ -1307,23 +1307,6 @@
     <col min="5" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="16.4416666666667" customWidth="1"/>
     <col min="8" max="8" width="20.2166666666667" customWidth="1"/>
-    <col min="9" max="9" width="11.6666666666667" customWidth="1"/>
-    <col min="10" max="10" width="27.775" customWidth="1"/>
-    <col min="11" max="11" width="17.775" customWidth="1"/>
-    <col min="12" max="12" width="32.775" customWidth="1"/>
-    <col min="13" max="14" width="20.2166666666667" customWidth="1"/>
-    <col min="15" max="15" width="24" customWidth="1"/>
-    <col min="16" max="17" width="21.4416666666667" customWidth="1"/>
-    <col min="18" max="18" width="15.2166666666667" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="16.4416666666667" customWidth="1"/>
-    <col min="21" max="21" width="19" customWidth="1"/>
-    <col min="22" max="22" width="15.2166666666667" customWidth="1"/>
-    <col min="23" max="23" width="20.2166666666667" customWidth="1"/>
-    <col min="24" max="24" width="11.6666666666667" customWidth="1"/>
-    <col min="25" max="25" width="20.2166666666667" customWidth="1"/>
-    <col min="26" max="27" width="17.775" customWidth="1"/>
-    <col min="28" max="28" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:8">
@@ -1352,7 +1335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:9">
+    <row r="2" s="2" customFormat="1" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1377,9 +1360,8 @@
       <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="6"/>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:9">
+    <row r="3" s="2" customFormat="1" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1404,9 +1386,8 @@
       <c r="H3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="7"/>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:9">
+    <row r="4" s="2" customFormat="1" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1431,9 +1412,8 @@
       <c r="H4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="7"/>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:9">
+    <row r="5" s="2" customFormat="1" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1458,9 +1438,8 @@
       <c r="H5" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="7"/>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:9">
+    <row r="6" s="2" customFormat="1" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1485,9 +1464,8 @@
       <c r="H6" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="7"/>
     </row>
-    <row r="7" s="3" customFormat="1" ht="68.25" spans="1:9">
+    <row r="7" s="3" customFormat="1" ht="68.25" spans="1:8">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
@@ -1512,7 +1490,6 @@
       <c r="H7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="10" t="s">
@@ -1721,214 +1698,6 @@
       <c r="H15">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="10"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="10"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="10"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="10"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="10"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="10"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="10"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="10"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="10"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="10"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="10"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="10"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="10"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="10"/>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="10"/>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="10"/>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="10"/>
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="10"/>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="10"/>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="10"/>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="10"/>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="10"/>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="10"/>
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="10"/>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="10"/>
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="10"/>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="10"/>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="10"/>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="10"/>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="10"/>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="10"/>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="10"/>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="10"/>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="10"/>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="10"/>
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="10"/>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="10"/>
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="10"/>
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="10"/>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="10"/>
-      <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="10"/>
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="10"/>
-      <c r="D61" s="10"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="10"/>
-      <c r="D62" s="10"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="10"/>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="10"/>
-      <c r="D64" s="10"/>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="10"/>
-      <c r="D66" s="10"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="10"/>
-      <c r="D67" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>